<commit_message>
Script to generate all results
</commit_message>
<xml_diff>
--- a/bench/results.xlsx
+++ b/bench/results.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akashlevy/Documents/NEM-Relay-CAD/bench/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ADA43A8-2A47-5547-9E4B-56495E3E061B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4424B9E1-2041-464B-9559-390F328DF7A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" activeTab="1" xr2:uid="{64AF3E00-AF30-AB47-A1E9-A89BC26FAE70}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{64AF3E00-AF30-AB47-A1E9-A89BC26FAE70}"/>
   </bookViews>
   <sheets>
-    <sheet name="Area Minimized" sheetId="1" r:id="rId1"/>
+    <sheet name="Area Minimized Results" sheetId="1" r:id="rId1"/>
     <sheet name="Area Plot" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -114,9 +114,6 @@
     <t>S-&gt;Z Energy (nJ)</t>
   </si>
   <si>
-    <t>Leakage Power (nW)</t>
-  </si>
-  <si>
     <t>CMOS Area (um^2)</t>
   </si>
   <si>
@@ -139,6 +136,9 @@
   </si>
   <si>
     <t>10-input 8b Mux</t>
+  </si>
+  <si>
+    <t>Leakage Power (W)</t>
   </si>
 </sst>
 </file>
@@ -182,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -190,6 +190,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -500,6 +503,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Area (a.u.)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1474,9 +1532,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CED39ECA-0ECC-3E44-A9C9-9795C2C70BB5}">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C35" sqref="C35:M35"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14:M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1553,13 +1611,26 @@
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" t="s">
-        <v>25</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="C6" s="5">
+        <v>8.9500000000000001E-10</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="1">
         <v>14.6412</v>
@@ -1578,7 +1649,7 @@
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="1">
         <v>0</v>
@@ -1623,13 +1694,24 @@
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" t="s">
-        <v>25</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="1">
         <v>29.282399999999999</v>
@@ -1648,7 +1730,7 @@
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" s="1">
         <v>0</v>
@@ -1693,13 +1775,24 @@
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" t="s">
-        <v>25</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" s="1">
         <v>80.262</v>
@@ -1718,7 +1811,7 @@
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C22" s="1">
         <v>0</v>
@@ -1796,13 +1889,24 @@
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" t="s">
-        <v>25</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C28" s="1">
         <v>0.5292</v>
@@ -1821,7 +1925,7 @@
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29" s="1">
         <f>3.78*3.78*2</f>
@@ -1900,13 +2004,24 @@
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
       <c r="B34" t="s">
-        <v>25</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
       <c r="B35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C35" s="1">
         <v>3.8807999999999998</v>
@@ -1925,7 +2040,7 @@
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
       <c r="B36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C36" s="1">
         <f>3.78*3.78*4</f>
@@ -2004,13 +2119,24 @@
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
       <c r="B41" t="s">
-        <v>25</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="4"/>
       <c r="B42" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C42" s="1">
         <v>13.935600000000001</v>
@@ -2029,7 +2155,7 @@
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="4"/>
       <c r="B43" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C43" s="1">
         <f>3.78*3.78*10</f>
@@ -2058,14 +2184,20 @@
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="24">
     <mergeCell ref="A37:A43"/>
     <mergeCell ref="C42:M42"/>
     <mergeCell ref="C43:M43"/>
+    <mergeCell ref="C6:M6"/>
+    <mergeCell ref="C13:M13"/>
+    <mergeCell ref="C20:M20"/>
+    <mergeCell ref="C27:M27"/>
+    <mergeCell ref="C34:M34"/>
+    <mergeCell ref="C41:M41"/>
     <mergeCell ref="A23:A29"/>
     <mergeCell ref="C28:M28"/>
     <mergeCell ref="C29:M29"/>
@@ -2088,62 +2220,77 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74385724-B559-854F-A5A1-4764DD491808}">
-  <dimension ref="A10:C13"/>
+  <dimension ref="A10:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>0</v>
       </c>
       <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
         <v>29</v>
       </c>
-      <c r="C10" t="s">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="B11">
+        <f>'Area Minimized Results'!C7</f>
+        <v>14.6412</v>
+      </c>
+      <c r="C11">
+        <f>'Area Minimized Results'!C28</f>
+        <v>0.5292</v>
+      </c>
+      <c r="D11">
+        <f>B11/C11</f>
+        <v>27.666666666666664</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>31</v>
       </c>
-      <c r="B11">
-        <f>'Area Minimized'!C7</f>
-        <v>14.6412</v>
-      </c>
-      <c r="C11">
-        <f>'Area Minimized'!C28</f>
-        <v>0.5292</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="B12">
+        <f>'Area Minimized Results'!C14</f>
+        <v>29.282399999999999</v>
+      </c>
+      <c r="C12">
+        <f>'Area Minimized Results'!C35</f>
+        <v>3.8807999999999998</v>
+      </c>
+      <c r="D12">
+        <f>B12/C12</f>
+        <v>7.5454545454545459</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>32</v>
       </c>
-      <c r="B12">
-        <f>'Area Minimized'!C14</f>
-        <v>29.282399999999999</v>
-      </c>
-      <c r="C12">
-        <f>'Area Minimized'!C35</f>
-        <v>3.8807999999999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>33</v>
-      </c>
       <c r="B13">
-        <f>'Area Minimized'!C21</f>
+        <f>'Area Minimized Results'!C21</f>
         <v>80.262</v>
       </c>
       <c r="C13">
-        <f>'Area Minimized'!C42</f>
+        <f>'Area Minimized Results'!C42</f>
         <v>13.935600000000001</v>
+      </c>
+      <c r="D13">
+        <f>B13/C13</f>
+        <v>5.7594936708860756</v>
       </c>
     </row>
   </sheetData>

</xml_diff>